<commit_message>
create first to first, second to second and second neighbourhood connection
</commit_message>
<xml_diff>
--- a/res_data/ES_result_table.xlsx
+++ b/res_data/ES_result_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huangcheng/Documents/ESBasedonSimilarity/res_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3673F8-3CB9-0646-884B-39F61D6846D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DC0A17-B6B8-9B42-9B11-DEF2863BCA0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" xr2:uid="{FAAE979D-3772-8244-8643-94FA117C2567}"/>
   </bookViews>
@@ -536,7 +536,7 @@
   <dimension ref="A1:O85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q69" sqref="Q69"/>
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2375,6 +2375,32 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A75:G75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="A60:G60"/>
+    <mergeCell ref="A61:G61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="A45:G45"/>
     <mergeCell ref="I75:O75"/>
     <mergeCell ref="J76:K76"/>
     <mergeCell ref="L76:M76"/>
@@ -2384,32 +2410,6 @@
     <mergeCell ref="J62:K62"/>
     <mergeCell ref="L62:M62"/>
     <mergeCell ref="N62:O62"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="A45:G45"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A15:G15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="A75:G75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="A60:G60"/>
-    <mergeCell ref="A61:G61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="F62:G62"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
complete graph dim 100 result
</commit_message>
<xml_diff>
--- a/res_data/ES_result_table.xlsx
+++ b/res_data/ES_result_table.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huangcheng/Documents/ESBasedonSimilarity/res_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DC0A17-B6B8-9B42-9B11-DEF2863BCA0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B855696-B3CB-B344-9D54-2F6294A4CD25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" xr2:uid="{FAAE979D-3772-8244-8643-94FA117C2567}"/>
+    <workbookView xWindow="3300" yWindow="-21100" windowWidth="22920" windowHeight="21100" xr2:uid="{FAAE979D-3772-8244-8643-94FA117C2567}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="21">
   <si>
     <t>dbpedia</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -109,6 +109,18 @@
     <t>Entropy Based Method(distmult)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Variance Based Method(transe, complete graph extract)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entropye Based Method(transe, complete graph extract, dim= 50)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Entropye Based Method(transe, complete graph extract, dim= 100)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -170,7 +182,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -205,6 +217,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -533,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B883A06B-C0CF-1844-AFD4-3454C5583175}">
-  <dimension ref="A1:O85"/>
+  <dimension ref="A1:O148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H64" sqref="H64"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G130" sqref="F130:G130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -545,30 +569,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="14" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="14" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="15"/>
+      <c r="G2" s="19"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8">
@@ -777,29 +801,29 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="14" t="s">
+      <c r="C16" s="19"/>
+      <c r="D16" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="14" t="s">
+      <c r="E16" s="19"/>
+      <c r="F16" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="15"/>
+      <c r="G16" s="19"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="1"/>
@@ -1007,40 +1031,40 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="14" t="s">
+      <c r="C32" s="19"/>
+      <c r="D32" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="15"/>
-      <c r="F32" s="14" t="s">
+      <c r="E32" s="19"/>
+      <c r="F32" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G32" s="15"/>
+      <c r="G32" s="19"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="8"/>
@@ -1248,29 +1272,29 @@
       </c>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="14" t="s">
+      <c r="A45" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B45" s="15"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="19"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="B46" s="14" t="s">
+      <c r="B46" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C46" s="15"/>
-      <c r="D46" s="14" t="s">
+      <c r="C46" s="19"/>
+      <c r="D46" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E46" s="15"/>
-      <c r="F46" s="14" t="s">
+      <c r="E46" s="19"/>
+      <c r="F46" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G46" s="15"/>
+      <c r="G46" s="19"/>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="8"/>
@@ -1478,70 +1502,70 @@
       </c>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="14" t="s">
+      <c r="A60" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B60" s="15"/>
-      <c r="C60" s="15"/>
-      <c r="D60" s="15"/>
-      <c r="E60" s="15"/>
-      <c r="F60" s="15"/>
-      <c r="G60" s="15"/>
-      <c r="I60" s="14" t="s">
+      <c r="B60" s="19"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="19"/>
+      <c r="G60" s="19"/>
+      <c r="I60" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J60" s="15"/>
-      <c r="K60" s="15"/>
-      <c r="L60" s="15"/>
-      <c r="M60" s="15"/>
-      <c r="N60" s="15"/>
-      <c r="O60" s="15"/>
+      <c r="J60" s="19"/>
+      <c r="K60" s="19"/>
+      <c r="L60" s="19"/>
+      <c r="M60" s="19"/>
+      <c r="N60" s="19"/>
+      <c r="O60" s="19"/>
     </row>
     <row r="61" spans="1:15">
-      <c r="A61" s="14" t="s">
+      <c r="A61" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B61" s="15"/>
-      <c r="C61" s="15"/>
-      <c r="D61" s="15"/>
-      <c r="E61" s="15"/>
-      <c r="F61" s="15"/>
-      <c r="G61" s="15"/>
-      <c r="I61" s="14" t="s">
+      <c r="B61" s="19"/>
+      <c r="C61" s="19"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="19"/>
+      <c r="G61" s="19"/>
+      <c r="I61" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="J61" s="15"/>
-      <c r="K61" s="15"/>
-      <c r="L61" s="15"/>
-      <c r="M61" s="15"/>
-      <c r="N61" s="15"/>
-      <c r="O61" s="15"/>
+      <c r="J61" s="19"/>
+      <c r="K61" s="19"/>
+      <c r="L61" s="19"/>
+      <c r="M61" s="19"/>
+      <c r="N61" s="19"/>
+      <c r="O61" s="19"/>
     </row>
     <row r="62" spans="1:15">
-      <c r="B62" s="14" t="s">
+      <c r="B62" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C62" s="15"/>
-      <c r="D62" s="14" t="s">
+      <c r="C62" s="19"/>
+      <c r="D62" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E62" s="15"/>
-      <c r="F62" s="14" t="s">
+      <c r="E62" s="19"/>
+      <c r="F62" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G62" s="15"/>
-      <c r="J62" s="14" t="s">
+      <c r="G62" s="19"/>
+      <c r="J62" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="K62" s="15"/>
-      <c r="L62" s="14" t="s">
+      <c r="K62" s="19"/>
+      <c r="L62" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="M62" s="15"/>
-      <c r="N62" s="14" t="s">
+      <c r="M62" s="19"/>
+      <c r="N62" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="O62" s="15"/>
+      <c r="O62" s="19"/>
     </row>
     <row r="63" spans="1:15">
       <c r="A63" s="10"/>
@@ -1936,50 +1960,50 @@
       </c>
     </row>
     <row r="75" spans="1:15">
-      <c r="A75" s="14" t="s">
+      <c r="A75" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B75" s="15"/>
-      <c r="C75" s="15"/>
-      <c r="D75" s="15"/>
-      <c r="E75" s="15"/>
-      <c r="F75" s="15"/>
-      <c r="G75" s="15"/>
-      <c r="I75" s="14" t="s">
+      <c r="B75" s="19"/>
+      <c r="C75" s="19"/>
+      <c r="D75" s="19"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="19"/>
+      <c r="G75" s="19"/>
+      <c r="I75" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="J75" s="15"/>
-      <c r="K75" s="15"/>
-      <c r="L75" s="15"/>
-      <c r="M75" s="15"/>
-      <c r="N75" s="15"/>
-      <c r="O75" s="15"/>
+      <c r="J75" s="19"/>
+      <c r="K75" s="19"/>
+      <c r="L75" s="19"/>
+      <c r="M75" s="19"/>
+      <c r="N75" s="19"/>
+      <c r="O75" s="19"/>
     </row>
     <row r="76" spans="1:15">
-      <c r="B76" s="14" t="s">
+      <c r="B76" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C76" s="15"/>
-      <c r="D76" s="14" t="s">
+      <c r="C76" s="19"/>
+      <c r="D76" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E76" s="15"/>
-      <c r="F76" s="14" t="s">
+      <c r="E76" s="19"/>
+      <c r="F76" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G76" s="15"/>
-      <c r="J76" s="14" t="s">
+      <c r="G76" s="19"/>
+      <c r="J76" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="K76" s="15"/>
-      <c r="L76" s="14" t="s">
+      <c r="K76" s="19"/>
+      <c r="L76" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="M76" s="15"/>
-      <c r="N76" s="14" t="s">
+      <c r="M76" s="19"/>
+      <c r="N76" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="O76" s="15"/>
+      <c r="O76" s="19"/>
     </row>
     <row r="77" spans="1:15">
       <c r="A77" s="10"/>
@@ -2373,8 +2397,1388 @@
         <v>0.38800000000000001</v>
       </c>
     </row>
+    <row r="92" spans="1:15">
+      <c r="A92" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B92" s="19"/>
+      <c r="C92" s="19"/>
+      <c r="D92" s="19"/>
+      <c r="E92" s="19"/>
+      <c r="F92" s="19"/>
+      <c r="G92" s="19"/>
+      <c r="I92" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="J92" s="19"/>
+      <c r="K92" s="19"/>
+      <c r="L92" s="19"/>
+      <c r="M92" s="19"/>
+      <c r="N92" s="19"/>
+      <c r="O92" s="19"/>
+    </row>
+    <row r="93" spans="1:15">
+      <c r="A93" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B93" s="19"/>
+      <c r="C93" s="19"/>
+      <c r="D93" s="19"/>
+      <c r="E93" s="19"/>
+      <c r="F93" s="19"/>
+      <c r="G93" s="19"/>
+      <c r="I93" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="J93" s="19"/>
+      <c r="K93" s="19"/>
+      <c r="L93" s="19"/>
+      <c r="M93" s="19"/>
+      <c r="N93" s="19"/>
+      <c r="O93" s="19"/>
+    </row>
+    <row r="94" spans="1:15">
+      <c r="B94" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C94" s="19"/>
+      <c r="D94" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E94" s="19"/>
+      <c r="F94" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G94" s="19"/>
+      <c r="J94" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="K94" s="19"/>
+      <c r="L94" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="M94" s="19"/>
+      <c r="N94" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="O94" s="19"/>
+    </row>
+    <row r="95" spans="1:15">
+      <c r="A95" s="15"/>
+      <c r="B95" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C95" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D95" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E95" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F95" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G95" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I95" s="15"/>
+      <c r="J95" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="K95" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L95" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="M95" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N95" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="O95" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15">
+      <c r="A96" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B96" s="15">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C96" s="15">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="D96" s="15">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="E96" s="15">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="F96" s="15">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="G96" s="15">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="I96" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="J96" s="15">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="K96" s="15">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="L96" s="15">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="M96" s="15">
+        <v>0.496</v>
+      </c>
+      <c r="N96" s="15">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="O96" s="15">
+        <v>0.497</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15">
+      <c r="A97" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B97" s="15">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="C97" s="15">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="D97" s="15">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="E97" s="15">
+        <v>0.495</v>
+      </c>
+      <c r="F97" s="14">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="G97" s="14">
+        <v>0.497</v>
+      </c>
+      <c r="I97" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J97" s="15">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="K97" s="15">
+        <v>0.48299999999999998</v>
+      </c>
+      <c r="L97" s="15">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="M97" s="15">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="N97" s="14">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="O97" s="14">
+        <v>0.49299999999999999</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15">
+      <c r="A98" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B98" s="15">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="C98" s="15">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="D98" s="15">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="E98" s="15">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="F98" s="11">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G98" s="11">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="I98" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="J98" s="15">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="K98" s="15">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="L98" s="15">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="M98" s="15">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="N98" s="11">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="O98" s="11">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15">
+      <c r="A99" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B99" s="15">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="C99" s="15">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="D99" s="15">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="E99" s="15">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="F99" s="11">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="G99" s="11">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="I99" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J99" s="15">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="K99" s="15">
+        <v>0.47</v>
+      </c>
+      <c r="L99" s="15">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="M99" s="15">
+        <v>0.48199999999999998</v>
+      </c>
+      <c r="N99" s="11">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="O99" s="11">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15">
+      <c r="A100" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B100" s="15">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="C100" s="15">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="D100" s="15">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="E100" s="15">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="F100" s="11">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="G100" s="11">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="I100" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J100" s="15">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="K100" s="15">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="L100" s="15">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="M100" s="15">
+        <v>0.48</v>
+      </c>
+      <c r="N100" s="11">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="O100" s="11">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15">
+      <c r="A101" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B101" s="15">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C101" s="15">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="D101" s="15">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="E101" s="15">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="F101" s="15">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="G101" s="15">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="I101" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J101" s="15">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="K101" s="15">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="L101" s="15">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="M101" s="15">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="N101" s="15">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="O101" s="15">
+        <v>0.48899999999999999</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15">
+      <c r="A102" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B102" s="15">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="C102" s="15">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="D102" s="15">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="E102" s="15">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="F102" s="15">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="G102" s="15">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="I102" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="J102" s="15">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="K102" s="15">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="L102" s="15">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="M102" s="15">
+        <v>0.48</v>
+      </c>
+      <c r="N102" s="15">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="O102" s="15">
+        <v>0.49099999999999999</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15">
+      <c r="A103" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B103" s="15">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="C103" s="15">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="D103" s="15">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="E103" s="15">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="F103" s="15">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="G103" s="15">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="I103" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J103" s="15">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="K103" s="15">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="L103" s="15">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M103" s="15">
+        <v>0.48</v>
+      </c>
+      <c r="N103" s="15">
+        <v>0.22</v>
+      </c>
+      <c r="O103" s="15">
+        <v>0.36899999999999999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15">
+      <c r="A107" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B107" s="19"/>
+      <c r="C107" s="19"/>
+      <c r="D107" s="19"/>
+      <c r="E107" s="19"/>
+      <c r="F107" s="19"/>
+      <c r="G107" s="19"/>
+      <c r="I107" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="J107" s="19"/>
+      <c r="K107" s="19"/>
+      <c r="L107" s="19"/>
+      <c r="M107" s="19"/>
+      <c r="N107" s="19"/>
+      <c r="O107" s="19"/>
+    </row>
+    <row r="108" spans="1:15">
+      <c r="B108" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C108" s="19"/>
+      <c r="D108" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E108" s="19"/>
+      <c r="F108" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G108" s="19"/>
+      <c r="J108" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="K108" s="19"/>
+      <c r="L108" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="M108" s="19"/>
+      <c r="N108" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="O108" s="19"/>
+    </row>
+    <row r="109" spans="1:15">
+      <c r="A109" s="15"/>
+      <c r="B109" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C109" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D109" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E109" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F109" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G109" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I109" s="15"/>
+      <c r="J109" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="K109" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L109" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="M109" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N109" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="O109" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15">
+      <c r="A110" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B110" s="11">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="C110" s="11">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="D110" s="11">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="E110" s="11">
+        <v>0.39</v>
+      </c>
+      <c r="F110" s="11">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="G110" s="11">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="I110" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="J110" s="11">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="K110" s="11">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="L110" s="11">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="M110" s="11">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="N110" s="11">
+        <v>0.251</v>
+      </c>
+      <c r="O110" s="11">
+        <v>0.39500000000000002</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15">
+      <c r="A111" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B111" s="14">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="C111" s="14">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="D111" s="11">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="E111" s="11">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="F111" s="11">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="G111" s="11">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="I111" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J111" s="14">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="K111" s="14">
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="L111" s="11">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="M111" s="11">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="N111" s="11">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="O111" s="11">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15">
+      <c r="A112" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B112" s="11">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="C112" s="11">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="D112" s="11">
+        <v>0.249</v>
+      </c>
+      <c r="E112" s="11">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="F112" s="11">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="G112" s="11">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="I112" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="J112" s="11">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="K112" s="11">
+        <v>0.377</v>
+      </c>
+      <c r="L112" s="11">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="M112" s="11">
+        <v>0.37</v>
+      </c>
+      <c r="N112" s="11">
+        <v>0.247</v>
+      </c>
+      <c r="O112" s="11">
+        <v>0.39100000000000001</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15">
+      <c r="A113" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B113" s="11">
+        <v>0.214</v>
+      </c>
+      <c r="C113" s="11">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="D113" s="11">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="E113" s="11">
+        <v>0.374</v>
+      </c>
+      <c r="F113" s="11">
+        <v>0.23</v>
+      </c>
+      <c r="G113" s="11">
+        <v>0.39</v>
+      </c>
+      <c r="I113" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J113" s="11">
+        <v>0.223</v>
+      </c>
+      <c r="K113" s="11">
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="L113" s="11">
+        <v>0.246</v>
+      </c>
+      <c r="M113" s="11">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="N113" s="11">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="O113" s="11">
+        <v>0.38200000000000001</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15">
+      <c r="A114" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B114" s="11">
+        <v>0.19</v>
+      </c>
+      <c r="C114" s="11">
+        <v>0.34</v>
+      </c>
+      <c r="D114" s="11">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="E114" s="11">
+        <v>0.372</v>
+      </c>
+      <c r="F114" s="11">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="G114" s="11">
+        <v>0.36</v>
+      </c>
+      <c r="I114" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J114" s="11">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="K114" s="11">
+        <v>0.34</v>
+      </c>
+      <c r="L114" s="11">
+        <v>0.245</v>
+      </c>
+      <c r="M114" s="11">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="N114" s="11">
+        <v>0.245</v>
+      </c>
+      <c r="O114" s="11">
+        <v>0.38100000000000001</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15">
+      <c r="A115" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B115" s="11">
+        <v>0.183</v>
+      </c>
+      <c r="C115" s="11">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="D115" s="11">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="E115" s="11">
+        <v>0.375</v>
+      </c>
+      <c r="F115" s="11">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="G115" s="11">
+        <v>0.378</v>
+      </c>
+      <c r="I115" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J115" s="11">
+        <v>0.191</v>
+      </c>
+      <c r="K115" s="11">
+        <v>0.34</v>
+      </c>
+      <c r="L115" s="11">
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="M115" s="11">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="N115" s="11">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="O115" s="11">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15">
+      <c r="A116" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B116" s="11">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="C116" s="11">
+        <v>0.33</v>
+      </c>
+      <c r="D116" s="11">
+        <v>0.247</v>
+      </c>
+      <c r="E116" s="11">
+        <v>0.378</v>
+      </c>
+      <c r="F116" s="11">
+        <v>0.24</v>
+      </c>
+      <c r="G116" s="11">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="I116" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="J116" s="11">
+        <v>0.158</v>
+      </c>
+      <c r="K116" s="11">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="L116" s="11">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="M116" s="11">
+        <v>0.373</v>
+      </c>
+      <c r="N116" s="11">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="O116" s="11">
+        <v>0.39700000000000002</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15">
+      <c r="A117" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B117" s="11">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="C117" s="11">
+        <v>0.308</v>
+      </c>
+      <c r="D117" s="11">
+        <v>0.219</v>
+      </c>
+      <c r="E117" s="11">
+        <v>0.374</v>
+      </c>
+      <c r="F117" s="11">
+        <v>0.247</v>
+      </c>
+      <c r="G117" s="11">
+        <v>0.37</v>
+      </c>
+      <c r="I117" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J117" s="11">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="K117" s="11">
+        <v>0.309</v>
+      </c>
+      <c r="L117" s="11">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="M117" s="11">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="N117" s="11">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="O117" s="11">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15">
+      <c r="A122" s="18"/>
+      <c r="B122" s="19"/>
+      <c r="C122" s="19"/>
+      <c r="D122" s="19"/>
+      <c r="E122" s="19"/>
+      <c r="F122" s="19"/>
+      <c r="G122" s="19"/>
+    </row>
+    <row r="123" spans="1:15">
+      <c r="A123" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B123" s="19"/>
+      <c r="C123" s="19"/>
+      <c r="D123" s="19"/>
+      <c r="E123" s="19"/>
+      <c r="F123" s="19"/>
+      <c r="G123" s="19"/>
+    </row>
+    <row r="124" spans="1:15">
+      <c r="A124" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B124" s="19"/>
+      <c r="C124" s="19"/>
+      <c r="D124" s="19"/>
+      <c r="E124" s="19"/>
+      <c r="F124" s="19"/>
+      <c r="G124" s="19"/>
+    </row>
+    <row r="125" spans="1:15">
+      <c r="B125" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C125" s="19"/>
+      <c r="D125" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E125" s="19"/>
+      <c r="F125" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G125" s="19"/>
+    </row>
+    <row r="126" spans="1:15">
+      <c r="A126" s="17"/>
+      <c r="B126" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C126" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D126" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E126" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F126" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G126" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15">
+      <c r="A127" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B127" s="11">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="C127" s="11">
+        <v>0.48199999999999998</v>
+      </c>
+      <c r="D127" s="11">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="E127" s="11">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="F127" s="11">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="G127" s="11">
+        <v>0.48299999999999998</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15">
+      <c r="A128" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B128" s="11">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="C128" s="11">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="D128" s="11">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="E128" s="11">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="F128" s="11">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G128" s="11">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7">
+      <c r="A129" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B129" s="11">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="C129" s="11">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="D129" s="11">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E129" s="11">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="F129" s="11">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="G129" s="11">
+        <v>0.48599999999999999</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7">
+      <c r="A130" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B130" s="11">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="C130" s="11">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="D130" s="11">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="E130" s="11">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="F130" s="16">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="G130" s="16">
+        <v>0.48799999999999999</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7">
+      <c r="A131" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B131" s="11">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="C131" s="11">
+        <v>0.47</v>
+      </c>
+      <c r="D131" s="11">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="E131" s="11">
+        <v>0.48199999999999998</v>
+      </c>
+      <c r="F131" s="11">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="G131" s="11">
+        <v>0.47799999999999998</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7">
+      <c r="A132" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B132" s="11">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="C132" s="11">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="D132" s="11">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="E132" s="11">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="F132" s="11">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="G132" s="11">
+        <v>0.48499999999999999</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7">
+      <c r="A133" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B133" s="11">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="C133" s="11">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="D133" s="11">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="E133" s="11">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="F133" s="11">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="G133" s="11">
+        <v>0.47399999999999998</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7">
+      <c r="A134" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B134" s="11">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C134" s="11">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="D134" s="11">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="E134" s="11">
+        <v>0.48199999999999998</v>
+      </c>
+      <c r="F134" s="11">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G134" s="11">
+        <v>0.47399999999999998</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7">
+      <c r="A138" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B138" s="19"/>
+      <c r="C138" s="19"/>
+      <c r="D138" s="19"/>
+      <c r="E138" s="19"/>
+      <c r="F138" s="19"/>
+      <c r="G138" s="19"/>
+    </row>
+    <row r="139" spans="1:7">
+      <c r="B139" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C139" s="19"/>
+      <c r="D139" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E139" s="19"/>
+      <c r="F139" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G139" s="19"/>
+    </row>
+    <row r="140" spans="1:7">
+      <c r="A140" s="17"/>
+      <c r="B140" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C140" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D140" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E140" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F140" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G140" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7">
+      <c r="A141" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B141" s="11">
+        <v>0.246</v>
+      </c>
+      <c r="C141" s="11">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="D141" s="11">
+        <v>0.247</v>
+      </c>
+      <c r="E141" s="11">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="F141" s="11">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="G141" s="11">
+        <v>0.40699999999999997</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7">
+      <c r="A142" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B142" s="16">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="C142" s="16">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="D142" s="11">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="E142" s="11">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="F142" s="11">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="G142" s="11">
+        <v>0.40799999999999997</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7">
+      <c r="A143" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B143" s="11">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="C143" s="11">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="D143" s="11">
+        <v>0.26</v>
+      </c>
+      <c r="E143" s="11">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="F143" s="11">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="G143" s="11">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7">
+      <c r="A144" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B144" s="11">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="C144" s="11">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="D144" s="11">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="E144" s="11">
+        <v>0.378</v>
+      </c>
+      <c r="F144" s="11">
+        <v>0.27</v>
+      </c>
+      <c r="G144" s="11">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7">
+      <c r="A145" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B145" s="11">
+        <v>0.214</v>
+      </c>
+      <c r="C145" s="11">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="D145" s="11">
+        <v>0.26</v>
+      </c>
+      <c r="E145" s="11">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="F145" s="11">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="G145" s="11">
+        <v>0.38400000000000001</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7">
+      <c r="A146" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B146" s="11">
+        <v>0.219</v>
+      </c>
+      <c r="C146" s="11">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="D146" s="11">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="E146" s="11">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="F146" s="11">
+        <v>0.249</v>
+      </c>
+      <c r="G146" s="11">
+        <v>0.374</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7">
+      <c r="A147" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B147" s="11">
+        <v>0.183</v>
+      </c>
+      <c r="C147" s="11">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="D147" s="11">
+        <v>0.253</v>
+      </c>
+      <c r="E147" s="11">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="F147" s="11">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="G147" s="11">
+        <v>0.38100000000000001</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7">
+      <c r="A148" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B148" s="11">
+        <v>0.185</v>
+      </c>
+      <c r="C148" s="11">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="D148" s="11">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="E148" s="11">
+        <v>0.379</v>
+      </c>
+      <c r="F148" s="11">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="G148" s="11">
+        <v>0.38900000000000001</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="63">
+    <mergeCell ref="A138:G138"/>
+    <mergeCell ref="B139:C139"/>
+    <mergeCell ref="D139:E139"/>
+    <mergeCell ref="F139:G139"/>
     <mergeCell ref="A75:G75"/>
     <mergeCell ref="B76:C76"/>
     <mergeCell ref="D76:E76"/>
@@ -2410,6 +3814,30 @@
     <mergeCell ref="J62:K62"/>
     <mergeCell ref="L62:M62"/>
     <mergeCell ref="N62:O62"/>
+    <mergeCell ref="A92:G92"/>
+    <mergeCell ref="A93:G93"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="F94:G94"/>
+    <mergeCell ref="A107:G107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="F108:G108"/>
+    <mergeCell ref="A122:G122"/>
+    <mergeCell ref="A124:G124"/>
+    <mergeCell ref="B125:C125"/>
+    <mergeCell ref="D125:E125"/>
+    <mergeCell ref="F125:G125"/>
+    <mergeCell ref="I92:O92"/>
+    <mergeCell ref="I93:O93"/>
+    <mergeCell ref="J94:K94"/>
+    <mergeCell ref="L94:M94"/>
+    <mergeCell ref="N94:O94"/>
+    <mergeCell ref="I107:O107"/>
+    <mergeCell ref="J108:K108"/>
+    <mergeCell ref="L108:M108"/>
+    <mergeCell ref="N108:O108"/>
+    <mergeCell ref="A123:G123"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
wrong experiment result on esbm
</commit_message>
<xml_diff>
--- a/res_data/ES_result_table.xlsx
+++ b/res_data/ES_result_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huangcheng/Documents/ESBasedonSimilarity/res_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B855696-B3CB-B344-9D54-2F6294A4CD25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DAC9E1-B7D6-0144-A7E5-F09EA74CE8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="-21100" windowWidth="22920" windowHeight="21100" xr2:uid="{FAAE979D-3772-8244-8643-94FA117C2567}"/>
+    <workbookView xWindow="3280" yWindow="-18520" windowWidth="28800" windowHeight="16320" xr2:uid="{FAAE979D-3772-8244-8643-94FA117C2567}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="22">
   <si>
     <t>dbpedia</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -121,6 +121,10 @@
     <t>Entropye Based Method(transe, complete graph extract, dim= 100)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Entropye Based Method Wrong Experiment(transe,ESBM)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -182,7 +186,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -217,6 +221,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -557,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B883A06B-C0CF-1844-AFD4-3454C5583175}">
-  <dimension ref="A1:O148"/>
+  <dimension ref="A1:O179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G130" sqref="F130:G130"/>
+    <sheetView tabSelected="1" topLeftCell="A151" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J177" sqref="J177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -569,30 +579,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="18" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="18" t="s">
+      <c r="E2" s="21"/>
+      <c r="F2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="19"/>
+      <c r="G2" s="21"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8">
@@ -801,29 +811,29 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="18" t="s">
+      <c r="C16" s="21"/>
+      <c r="D16" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="18" t="s">
+      <c r="E16" s="21"/>
+      <c r="F16" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="19"/>
+      <c r="G16" s="21"/>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="1"/>
@@ -1031,40 +1041,40 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="18" t="s">
+      <c r="A31" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="18" t="s">
+      <c r="C32" s="21"/>
+      <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="19"/>
-      <c r="F32" s="18" t="s">
+      <c r="E32" s="21"/>
+      <c r="F32" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G32" s="19"/>
+      <c r="G32" s="21"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="8"/>
@@ -1272,29 +1282,29 @@
       </c>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="18" t="s">
+      <c r="A45" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B45" s="19"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="B46" s="18" t="s">
+      <c r="B46" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C46" s="19"/>
-      <c r="D46" s="18" t="s">
+      <c r="C46" s="21"/>
+      <c r="D46" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E46" s="19"/>
-      <c r="F46" s="18" t="s">
+      <c r="E46" s="21"/>
+      <c r="F46" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G46" s="19"/>
+      <c r="G46" s="21"/>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="8"/>
@@ -1502,70 +1512,70 @@
       </c>
     </row>
     <row r="60" spans="1:15">
-      <c r="A60" s="18" t="s">
+      <c r="A60" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B60" s="19"/>
-      <c r="C60" s="19"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="19"/>
-      <c r="F60" s="19"/>
-      <c r="G60" s="19"/>
-      <c r="I60" s="18" t="s">
+      <c r="B60" s="21"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="21"/>
+      <c r="F60" s="21"/>
+      <c r="G60" s="21"/>
+      <c r="I60" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="J60" s="19"/>
-      <c r="K60" s="19"/>
-      <c r="L60" s="19"/>
-      <c r="M60" s="19"/>
-      <c r="N60" s="19"/>
-      <c r="O60" s="19"/>
+      <c r="J60" s="21"/>
+      <c r="K60" s="21"/>
+      <c r="L60" s="21"/>
+      <c r="M60" s="21"/>
+      <c r="N60" s="21"/>
+      <c r="O60" s="21"/>
     </row>
     <row r="61" spans="1:15">
-      <c r="A61" s="18" t="s">
+      <c r="A61" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B61" s="19"/>
-      <c r="C61" s="19"/>
-      <c r="D61" s="19"/>
-      <c r="E61" s="19"/>
-      <c r="F61" s="19"/>
-      <c r="G61" s="19"/>
-      <c r="I61" s="18" t="s">
+      <c r="B61" s="21"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="21"/>
+      <c r="G61" s="21"/>
+      <c r="I61" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="J61" s="19"/>
-      <c r="K61" s="19"/>
-      <c r="L61" s="19"/>
-      <c r="M61" s="19"/>
-      <c r="N61" s="19"/>
-      <c r="O61" s="19"/>
+      <c r="J61" s="21"/>
+      <c r="K61" s="21"/>
+      <c r="L61" s="21"/>
+      <c r="M61" s="21"/>
+      <c r="N61" s="21"/>
+      <c r="O61" s="21"/>
     </row>
     <row r="62" spans="1:15">
-      <c r="B62" s="18" t="s">
+      <c r="B62" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C62" s="19"/>
-      <c r="D62" s="18" t="s">
+      <c r="C62" s="21"/>
+      <c r="D62" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E62" s="19"/>
-      <c r="F62" s="18" t="s">
+      <c r="E62" s="21"/>
+      <c r="F62" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G62" s="19"/>
-      <c r="J62" s="18" t="s">
+      <c r="G62" s="21"/>
+      <c r="J62" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K62" s="19"/>
-      <c r="L62" s="18" t="s">
+      <c r="K62" s="21"/>
+      <c r="L62" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="M62" s="19"/>
-      <c r="N62" s="18" t="s">
+      <c r="M62" s="21"/>
+      <c r="N62" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="O62" s="19"/>
+      <c r="O62" s="21"/>
     </row>
     <row r="63" spans="1:15">
       <c r="A63" s="10"/>
@@ -1960,50 +1970,50 @@
       </c>
     </row>
     <row r="75" spans="1:15">
-      <c r="A75" s="18" t="s">
+      <c r="A75" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B75" s="19"/>
-      <c r="C75" s="19"/>
-      <c r="D75" s="19"/>
-      <c r="E75" s="19"/>
-      <c r="F75" s="19"/>
-      <c r="G75" s="19"/>
-      <c r="I75" s="18" t="s">
+      <c r="B75" s="21"/>
+      <c r="C75" s="21"/>
+      <c r="D75" s="21"/>
+      <c r="E75" s="21"/>
+      <c r="F75" s="21"/>
+      <c r="G75" s="21"/>
+      <c r="I75" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="J75" s="19"/>
-      <c r="K75" s="19"/>
-      <c r="L75" s="19"/>
-      <c r="M75" s="19"/>
-      <c r="N75" s="19"/>
-      <c r="O75" s="19"/>
+      <c r="J75" s="21"/>
+      <c r="K75" s="21"/>
+      <c r="L75" s="21"/>
+      <c r="M75" s="21"/>
+      <c r="N75" s="21"/>
+      <c r="O75" s="21"/>
     </row>
     <row r="76" spans="1:15">
-      <c r="B76" s="18" t="s">
+      <c r="B76" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C76" s="19"/>
-      <c r="D76" s="18" t="s">
+      <c r="C76" s="21"/>
+      <c r="D76" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E76" s="19"/>
-      <c r="F76" s="18" t="s">
+      <c r="E76" s="21"/>
+      <c r="F76" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G76" s="19"/>
-      <c r="J76" s="18" t="s">
+      <c r="G76" s="21"/>
+      <c r="J76" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K76" s="19"/>
-      <c r="L76" s="18" t="s">
+      <c r="K76" s="21"/>
+      <c r="L76" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="M76" s="19"/>
-      <c r="N76" s="18" t="s">
+      <c r="M76" s="21"/>
+      <c r="N76" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="O76" s="19"/>
+      <c r="O76" s="21"/>
     </row>
     <row r="77" spans="1:15">
       <c r="A77" s="10"/>
@@ -2398,70 +2408,70 @@
       </c>
     </row>
     <row r="92" spans="1:15">
-      <c r="A92" s="18" t="s">
+      <c r="A92" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B92" s="19"/>
-      <c r="C92" s="19"/>
-      <c r="D92" s="19"/>
-      <c r="E92" s="19"/>
-      <c r="F92" s="19"/>
-      <c r="G92" s="19"/>
-      <c r="I92" s="18" t="s">
+      <c r="B92" s="21"/>
+      <c r="C92" s="21"/>
+      <c r="D92" s="21"/>
+      <c r="E92" s="21"/>
+      <c r="F92" s="21"/>
+      <c r="G92" s="21"/>
+      <c r="I92" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="J92" s="19"/>
-      <c r="K92" s="19"/>
-      <c r="L92" s="19"/>
-      <c r="M92" s="19"/>
-      <c r="N92" s="19"/>
-      <c r="O92" s="19"/>
+      <c r="J92" s="21"/>
+      <c r="K92" s="21"/>
+      <c r="L92" s="21"/>
+      <c r="M92" s="21"/>
+      <c r="N92" s="21"/>
+      <c r="O92" s="21"/>
     </row>
     <row r="93" spans="1:15">
-      <c r="A93" s="18" t="s">
+      <c r="A93" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B93" s="19"/>
-      <c r="C93" s="19"/>
-      <c r="D93" s="19"/>
-      <c r="E93" s="19"/>
-      <c r="F93" s="19"/>
-      <c r="G93" s="19"/>
-      <c r="I93" s="18" t="s">
+      <c r="B93" s="21"/>
+      <c r="C93" s="21"/>
+      <c r="D93" s="21"/>
+      <c r="E93" s="21"/>
+      <c r="F93" s="21"/>
+      <c r="G93" s="21"/>
+      <c r="I93" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="J93" s="19"/>
-      <c r="K93" s="19"/>
-      <c r="L93" s="19"/>
-      <c r="M93" s="19"/>
-      <c r="N93" s="19"/>
-      <c r="O93" s="19"/>
+      <c r="J93" s="21"/>
+      <c r="K93" s="21"/>
+      <c r="L93" s="21"/>
+      <c r="M93" s="21"/>
+      <c r="N93" s="21"/>
+      <c r="O93" s="21"/>
     </row>
     <row r="94" spans="1:15">
-      <c r="B94" s="18" t="s">
+      <c r="B94" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C94" s="19"/>
-      <c r="D94" s="18" t="s">
+      <c r="C94" s="21"/>
+      <c r="D94" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E94" s="19"/>
-      <c r="F94" s="18" t="s">
+      <c r="E94" s="21"/>
+      <c r="F94" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G94" s="19"/>
-      <c r="J94" s="18" t="s">
+      <c r="G94" s="21"/>
+      <c r="J94" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K94" s="19"/>
-      <c r="L94" s="18" t="s">
+      <c r="K94" s="21"/>
+      <c r="L94" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="M94" s="19"/>
-      <c r="N94" s="18" t="s">
+      <c r="M94" s="21"/>
+      <c r="N94" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="O94" s="19"/>
+      <c r="O94" s="21"/>
     </row>
     <row r="95" spans="1:15">
       <c r="A95" s="15"/>
@@ -2856,50 +2866,50 @@
       </c>
     </row>
     <row r="107" spans="1:15">
-      <c r="A107" s="18" t="s">
+      <c r="A107" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B107" s="19"/>
-      <c r="C107" s="19"/>
-      <c r="D107" s="19"/>
-      <c r="E107" s="19"/>
-      <c r="F107" s="19"/>
-      <c r="G107" s="19"/>
-      <c r="I107" s="18" t="s">
+      <c r="B107" s="21"/>
+      <c r="C107" s="21"/>
+      <c r="D107" s="21"/>
+      <c r="E107" s="21"/>
+      <c r="F107" s="21"/>
+      <c r="G107" s="21"/>
+      <c r="I107" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="J107" s="19"/>
-      <c r="K107" s="19"/>
-      <c r="L107" s="19"/>
-      <c r="M107" s="19"/>
-      <c r="N107" s="19"/>
-      <c r="O107" s="19"/>
+      <c r="J107" s="21"/>
+      <c r="K107" s="21"/>
+      <c r="L107" s="21"/>
+      <c r="M107" s="21"/>
+      <c r="N107" s="21"/>
+      <c r="O107" s="21"/>
     </row>
     <row r="108" spans="1:15">
-      <c r="B108" s="18" t="s">
+      <c r="B108" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C108" s="19"/>
-      <c r="D108" s="18" t="s">
+      <c r="C108" s="21"/>
+      <c r="D108" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E108" s="19"/>
-      <c r="F108" s="18" t="s">
+      <c r="E108" s="21"/>
+      <c r="F108" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G108" s="19"/>
-      <c r="J108" s="18" t="s">
+      <c r="G108" s="21"/>
+      <c r="J108" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="K108" s="19"/>
-      <c r="L108" s="18" t="s">
+      <c r="K108" s="21"/>
+      <c r="L108" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="M108" s="19"/>
-      <c r="N108" s="18" t="s">
+      <c r="M108" s="21"/>
+      <c r="N108" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="O108" s="19"/>
+      <c r="O108" s="21"/>
     </row>
     <row r="109" spans="1:15">
       <c r="A109" s="15"/>
@@ -3294,49 +3304,49 @@
       </c>
     </row>
     <row r="122" spans="1:15">
-      <c r="A122" s="18"/>
-      <c r="B122" s="19"/>
-      <c r="C122" s="19"/>
-      <c r="D122" s="19"/>
-      <c r="E122" s="19"/>
-      <c r="F122" s="19"/>
-      <c r="G122" s="19"/>
+      <c r="A122" s="20"/>
+      <c r="B122" s="21"/>
+      <c r="C122" s="21"/>
+      <c r="D122" s="21"/>
+      <c r="E122" s="21"/>
+      <c r="F122" s="21"/>
+      <c r="G122" s="21"/>
     </row>
     <row r="123" spans="1:15">
-      <c r="A123" s="18" t="s">
+      <c r="A123" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B123" s="19"/>
-      <c r="C123" s="19"/>
-      <c r="D123" s="19"/>
-      <c r="E123" s="19"/>
-      <c r="F123" s="19"/>
-      <c r="G123" s="19"/>
+      <c r="B123" s="21"/>
+      <c r="C123" s="21"/>
+      <c r="D123" s="21"/>
+      <c r="E123" s="21"/>
+      <c r="F123" s="21"/>
+      <c r="G123" s="21"/>
     </row>
     <row r="124" spans="1:15">
-      <c r="A124" s="18" t="s">
+      <c r="A124" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B124" s="19"/>
-      <c r="C124" s="19"/>
-      <c r="D124" s="19"/>
-      <c r="E124" s="19"/>
-      <c r="F124" s="19"/>
-      <c r="G124" s="19"/>
+      <c r="B124" s="21"/>
+      <c r="C124" s="21"/>
+      <c r="D124" s="21"/>
+      <c r="E124" s="21"/>
+      <c r="F124" s="21"/>
+      <c r="G124" s="21"/>
     </row>
     <row r="125" spans="1:15">
-      <c r="B125" s="18" t="s">
+      <c r="B125" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C125" s="19"/>
-      <c r="D125" s="18" t="s">
+      <c r="C125" s="21"/>
+      <c r="D125" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E125" s="19"/>
-      <c r="F125" s="18" t="s">
+      <c r="E125" s="21"/>
+      <c r="F125" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G125" s="19"/>
+      <c r="G125" s="21"/>
     </row>
     <row r="126" spans="1:15">
       <c r="A126" s="17"/>
@@ -3544,29 +3554,29 @@
       </c>
     </row>
     <row r="138" spans="1:7">
-      <c r="A138" s="18" t="s">
+      <c r="A138" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B138" s="19"/>
-      <c r="C138" s="19"/>
-      <c r="D138" s="19"/>
-      <c r="E138" s="19"/>
-      <c r="F138" s="19"/>
-      <c r="G138" s="19"/>
+      <c r="B138" s="21"/>
+      <c r="C138" s="21"/>
+      <c r="D138" s="21"/>
+      <c r="E138" s="21"/>
+      <c r="F138" s="21"/>
+      <c r="G138" s="21"/>
     </row>
     <row r="139" spans="1:7">
-      <c r="B139" s="18" t="s">
+      <c r="B139" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C139" s="19"/>
-      <c r="D139" s="18" t="s">
+      <c r="C139" s="21"/>
+      <c r="D139" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E139" s="19"/>
-      <c r="F139" s="18" t="s">
+      <c r="E139" s="21"/>
+      <c r="F139" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G139" s="19"/>
+      <c r="G139" s="21"/>
     </row>
     <row r="140" spans="1:7">
       <c r="A140" s="17"/>
@@ -3773,8 +3783,488 @@
         <v>0.38900000000000001</v>
       </c>
     </row>
+    <row r="154" spans="1:7">
+      <c r="A154" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B154" s="21"/>
+      <c r="C154" s="21"/>
+      <c r="D154" s="21"/>
+      <c r="E154" s="21"/>
+      <c r="F154" s="21"/>
+      <c r="G154" s="21"/>
+    </row>
+    <row r="155" spans="1:7">
+      <c r="A155" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B155" s="21"/>
+      <c r="C155" s="21"/>
+      <c r="D155" s="21"/>
+      <c r="E155" s="21"/>
+      <c r="F155" s="21"/>
+      <c r="G155" s="21"/>
+    </row>
+    <row r="156" spans="1:7">
+      <c r="B156" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C156" s="21"/>
+      <c r="D156" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E156" s="21"/>
+      <c r="F156" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G156" s="21"/>
+    </row>
+    <row r="157" spans="1:7">
+      <c r="A157" s="19"/>
+      <c r="B157" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C157" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D157" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E157" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F157" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G157" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7">
+      <c r="A158" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B158" s="11">
+        <v>0.3</v>
+      </c>
+      <c r="C158" s="11">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="D158" s="11">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E158" s="11">
+        <v>0.53300000000000003</v>
+      </c>
+      <c r="F158" s="11">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="G158" s="11">
+        <v>0.53600000000000003</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7">
+      <c r="A159" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B159" s="11">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="C159" s="11">
+        <v>0.52900000000000003</v>
+      </c>
+      <c r="D159" s="11">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="E159" s="11">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="F159" s="11">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="G159" s="11">
+        <v>0.53500000000000003</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7">
+      <c r="A160" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B160" s="11">
+        <v>0.307</v>
+      </c>
+      <c r="C160" s="11">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="D160" s="11">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="E160" s="11">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="F160" s="11">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="G160" s="11">
+        <v>0.53700000000000003</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7">
+      <c r="A161" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B161" s="11">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="C161" s="11">
+        <v>0.52</v>
+      </c>
+      <c r="D161" s="11">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="E161" s="11">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="F161" s="18">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="G161" s="18">
+        <v>0.53300000000000003</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7">
+      <c r="A162" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B162" s="11">
+        <v>0.3</v>
+      </c>
+      <c r="C162" s="11">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="D162" s="11">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="E162" s="11">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="F162" s="11">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="G162" s="11">
+        <v>0.53400000000000003</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7">
+      <c r="A163" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B163" s="11">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="C163" s="11">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="D163" s="11">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="E163" s="11">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="F163" s="11">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="G163" s="11">
+        <v>0.53500000000000003</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7">
+      <c r="A164" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B164" s="11">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="C164" s="11">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="D164" s="11">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="E164" s="11">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="F164" s="11">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="G164" s="11">
+        <v>0.53500000000000003</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7">
+      <c r="A165" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B165" s="11">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="C165" s="11">
+        <v>0.505</v>
+      </c>
+      <c r="D165" s="11">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="E165" s="11">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="F165" s="11">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="G165" s="11">
+        <v>0.53400000000000003</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7">
+      <c r="A169" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B169" s="21"/>
+      <c r="C169" s="21"/>
+      <c r="D169" s="21"/>
+      <c r="E169" s="21"/>
+      <c r="F169" s="21"/>
+      <c r="G169" s="21"/>
+    </row>
+    <row r="170" spans="1:7">
+      <c r="B170" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C170" s="21"/>
+      <c r="D170" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E170" s="21"/>
+      <c r="F170" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G170" s="21"/>
+    </row>
+    <row r="171" spans="1:7">
+      <c r="A171" s="19"/>
+      <c r="B171" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C171" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D171" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E171" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F171" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G171" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7">
+      <c r="A172" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B172" s="11">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="C172" s="11">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="D172" s="11">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="E172" s="11">
+        <v>0.42699999999999999</v>
+      </c>
+      <c r="F172" s="11">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="G172" s="11">
+        <v>0.42299999999999999</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7">
+      <c r="A173" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B173" s="18">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="C173" s="18">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="D173" s="11">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="E173" s="11">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="F173" s="11">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="G173" s="11">
+        <v>0.42799999999999999</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7">
+      <c r="A174" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B174" s="11">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="C174" s="11">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="D174" s="11">
+        <v>0.26100000000000001</v>
+      </c>
+      <c r="E174" s="11">
+        <v>0.43</v>
+      </c>
+      <c r="F174" s="11">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="G174" s="11">
+        <v>0.42799999999999999</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7">
+      <c r="A175" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B175" s="11">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="C175" s="11">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="D175" s="11">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="E175" s="11">
+        <v>0.43</v>
+      </c>
+      <c r="F175" s="11">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="G175" s="11">
+        <v>0.42599999999999999</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7">
+      <c r="A176" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B176" s="11">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="C176" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="D176" s="11">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="E176" s="11">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="F176" s="11">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="G176" s="11">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7">
+      <c r="A177" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B177" s="11">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="C177" s="11">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="D177" s="11">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="E177" s="11">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="F177" s="11">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="G177" s="11">
+        <v>0.41799999999999998</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7">
+      <c r="A178" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B178" s="11">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="C178" s="11">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="D178" s="11">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="E178" s="11">
+        <v>0.42</v>
+      </c>
+      <c r="F178" s="11">
+        <v>0.26</v>
+      </c>
+      <c r="G178" s="11">
+        <v>0.42099999999999999</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7">
+      <c r="A179" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B179" s="11">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="C179" s="11">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="D179" s="11">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="E179" s="11">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="F179" s="11">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="G179" s="11">
+        <v>0.42699999999999999</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="63">
+  <mergeCells count="72">
+    <mergeCell ref="A169:G169"/>
+    <mergeCell ref="B170:C170"/>
+    <mergeCell ref="D170:E170"/>
+    <mergeCell ref="F170:G170"/>
+    <mergeCell ref="A154:G154"/>
+    <mergeCell ref="A155:G155"/>
+    <mergeCell ref="B156:C156"/>
+    <mergeCell ref="D156:E156"/>
+    <mergeCell ref="F156:G156"/>
     <mergeCell ref="A138:G138"/>
     <mergeCell ref="B139:C139"/>
     <mergeCell ref="D139:E139"/>
@@ -3783,6 +4273,14 @@
     <mergeCell ref="B76:C76"/>
     <mergeCell ref="D76:E76"/>
     <mergeCell ref="F76:G76"/>
+    <mergeCell ref="A92:G92"/>
+    <mergeCell ref="A93:G93"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="F94:G94"/>
+    <mergeCell ref="A107:G107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="D108:E108"/>
     <mergeCell ref="A60:G60"/>
     <mergeCell ref="A61:G61"/>
     <mergeCell ref="B62:C62"/>
@@ -3805,29 +4303,19 @@
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="F32:G32"/>
     <mergeCell ref="A45:G45"/>
-    <mergeCell ref="I75:O75"/>
-    <mergeCell ref="J76:K76"/>
-    <mergeCell ref="L76:M76"/>
-    <mergeCell ref="N76:O76"/>
     <mergeCell ref="I60:O60"/>
     <mergeCell ref="I61:O61"/>
     <mergeCell ref="J62:K62"/>
     <mergeCell ref="L62:M62"/>
     <mergeCell ref="N62:O62"/>
-    <mergeCell ref="A92:G92"/>
-    <mergeCell ref="A93:G93"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="F94:G94"/>
-    <mergeCell ref="A107:G107"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="F108:G108"/>
-    <mergeCell ref="A122:G122"/>
     <mergeCell ref="A124:G124"/>
     <mergeCell ref="B125:C125"/>
     <mergeCell ref="D125:E125"/>
     <mergeCell ref="F125:G125"/>
+    <mergeCell ref="I75:O75"/>
+    <mergeCell ref="J76:K76"/>
+    <mergeCell ref="L76:M76"/>
+    <mergeCell ref="N76:O76"/>
     <mergeCell ref="I92:O92"/>
     <mergeCell ref="I93:O93"/>
     <mergeCell ref="J94:K94"/>
@@ -3838,6 +4326,8 @@
     <mergeCell ref="L108:M108"/>
     <mergeCell ref="N108:O108"/>
     <mergeCell ref="A123:G123"/>
+    <mergeCell ref="F108:G108"/>
+    <mergeCell ref="A122:G122"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>